<commit_message>
changed to one col and added button to training page
</commit_message>
<xml_diff>
--- a/TrainingMatrix.xlsx
+++ b/TrainingMatrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mado\Documents\RoleRelatedTraining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mado\Documents\C_Desktop\roleRelatedTraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0BC003-CA10-40C8-913A-6172BEF22F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF9DFA-6B60-407A-A58C-887D3170717C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12456" xr2:uid="{89DB8824-010E-4172-8BDD-760FF30D7ADC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{89DB8824-010E-4172-8BDD-760FF30D7ADC}"/>
   </bookViews>
   <sheets>
     <sheet name="TrainingMatrix" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="126">
   <si>
     <t>Category</t>
   </si>
@@ -287,9 +287,6 @@
     <t>Introduction to the basic personalization and navigation settings of Infor LN.</t>
   </si>
   <si>
-    <t>INFOR LN LOOK AND FEEL 1 &amp; 2</t>
-  </si>
-  <si>
     <t>AP INVOICE REGISTRATION</t>
   </si>
   <si>
@@ -311,12 +308,6 @@
     <t>ACCOUNT MATCHING</t>
   </si>
   <si>
-    <t>ACP MONITORING</t>
-  </si>
-  <si>
-    <t>ACR MONITORING</t>
-  </si>
-  <si>
     <t>AUTOMATIC PAYMENTS</t>
   </si>
   <si>
@@ -413,13 +404,13 @@
     <t>YELLOWSTAR (WAREHOUSE RECEIPT)</t>
   </si>
   <si>
-    <t>Dates</t>
-  </si>
-  <si>
-    <t>01/03/2025, 04/03/2026</t>
-  </si>
-  <si>
-    <t>04/03/2025, 01/04/2025, 06/05/2025, 03/06/2025, 01/07/2025, 05/08/2025, 02/09/2025, 07/10/2025, 04/11/2025, 02/12/2025</t>
+    <t>INFOR LN LOOK AND FEEL</t>
+  </si>
+  <si>
+    <t>ACCOUNTS PAYABLE MONITORING</t>
+  </si>
+  <si>
+    <t>ACCOUNTS RECEIVABLE MONITORING</t>
   </si>
 </sst>
 </file>
@@ -909,11 +900,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1289,20 +1277,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499923C8-67A8-4D05-B09A-9EA7B6DF0BF0}">
-  <dimension ref="A1:AP58"/>
+  <dimension ref="A1:AO58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="56.85546875" customWidth="1"/>
+    <col min="3" max="3" width="56.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1313,135 +1301,132 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AG1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AH1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AJ1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AK1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AL1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AM1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AN1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>128</v>
+      <c r="D2" t="s">
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>42</v>
@@ -1500,7 +1485,7 @@
       <c r="W2" t="s">
         <v>42</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>42</v>
       </c>
       <c r="Z2" t="s">
@@ -1548,69 +1533,64 @@
       <c r="AN2" t="s">
         <v>42</v>
       </c>
-      <c r="AO2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
         <v>42</v>
       </c>
       <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+      <c r="U5" t="s">
         <v>42</v>
       </c>
       <c r="V5" t="s">
@@ -1619,7 +1599,7 @@
       <c r="W5" t="s">
         <v>42</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AF5" t="s">
         <v>42</v>
       </c>
       <c r="AG5" t="s">
@@ -1628,28 +1608,27 @@
       <c r="AH5" t="s">
         <v>42</v>
       </c>
-      <c r="AI5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AM5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
       <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>42</v>
       </c>
       <c r="I6" t="s">
@@ -1664,10 +1643,10 @@
       <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="M6" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="N6" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" t="s">
         <v>42</v>
       </c>
       <c r="V6" t="s">
@@ -1676,13 +1655,13 @@
       <c r="W6" t="s">
         <v>42</v>
       </c>
-      <c r="X6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC6" t="s">
+      <c r="Y6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" t="s">
         <v>42</v>
       </c>
       <c r="AF6" t="s">
@@ -1697,58 +1676,55 @@
       <c r="AI6" t="s">
         <v>42</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AL6" t="s">
         <v>42</v>
       </c>
       <c r="AM6" t="s">
         <v>42</v>
       </c>
-      <c r="AN6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
+      <c r="U9" t="s">
         <v>42</v>
       </c>
       <c r="V9" t="s">
@@ -1757,37 +1733,36 @@
       <c r="W9" t="s">
         <v>42</v>
       </c>
-      <c r="X9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
       <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>42</v>
+      </c>
+      <c r="U10" t="s">
         <v>42</v>
       </c>
       <c r="V10" t="s">
@@ -1796,40 +1771,39 @@
       <c r="W10" t="s">
         <v>42</v>
       </c>
-      <c r="X10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="Y10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL10" t="s">
         <v>42</v>
       </c>
       <c r="AM10" t="s">
         <v>42</v>
       </c>
-      <c r="AN10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" t="s">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
         <v>42</v>
       </c>
       <c r="G11" t="s">
         <v>42</v>
       </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+      <c r="U11" t="s">
         <v>42</v>
       </c>
       <c r="V11" t="s">
@@ -1838,40 +1812,39 @@
       <c r="W11" t="s">
         <v>42</v>
       </c>
-      <c r="X11" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z11" t="s">
+      <c r="Y11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL11" t="s">
         <v>42</v>
       </c>
       <c r="AM11" t="s">
         <v>42</v>
       </c>
-      <c r="AN11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
+      <c r="U12" t="s">
         <v>42</v>
       </c>
       <c r="V12" t="s">
@@ -1880,34 +1853,33 @@
       <c r="W12" t="s">
         <v>42</v>
       </c>
-      <c r="X12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" t="s">
         <v>42</v>
       </c>
       <c r="V13" t="s">
@@ -1916,34 +1888,33 @@
       <c r="W13" t="s">
         <v>42</v>
       </c>
-      <c r="X13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
+        <v>42</v>
+      </c>
+      <c r="U14" t="s">
         <v>42</v>
       </c>
       <c r="V14" t="s">
@@ -1952,37 +1923,36 @@
       <c r="W14" t="s">
         <v>42</v>
       </c>
-      <c r="X14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z14" t="s">
+      <c r="Y14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL14" t="s">
         <v>42</v>
       </c>
       <c r="AM14" t="s">
         <v>42</v>
       </c>
-      <c r="AN14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" t="s">
+        <v>42</v>
+      </c>
+      <c r="U15" t="s">
         <v>42</v>
       </c>
       <c r="V15" t="s">
@@ -1991,61 +1961,61 @@
       <c r="W15" t="s">
         <v>42</v>
       </c>
-      <c r="X15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
         <v>57</v>
       </c>
-      <c r="E18" t="s">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
         <v>42</v>
       </c>
       <c r="G18" t="s">
         <v>42</v>
       </c>
-      <c r="H18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" t="s">
+      <c r="J18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U18" t="s">
         <v>42</v>
       </c>
       <c r="V18" t="s">
@@ -2054,36 +2024,36 @@
       <c r="W18" t="s">
         <v>42</v>
       </c>
-      <c r="X18" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="E19" t="s">
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
         <v>42</v>
       </c>
       <c r="G19" t="s">
         <v>42</v>
       </c>
-      <c r="H19" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="J19" t="s">
+        <v>42</v>
+      </c>
+      <c r="U19" t="s">
         <v>42</v>
       </c>
       <c r="V19" t="s">
@@ -2092,33 +2062,33 @@
       <c r="W19" t="s">
         <v>42</v>
       </c>
-      <c r="X19" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="E20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" t="s">
-        <v>42</v>
-      </c>
-      <c r="K20" t="s">
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" t="s">
+        <v>42</v>
+      </c>
+      <c r="U20" t="s">
         <v>42</v>
       </c>
       <c r="V20" t="s">
@@ -2127,27 +2097,27 @@
       <c r="W20" t="s">
         <v>42</v>
       </c>
-      <c r="X20" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y20" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="K21" t="s">
+      <c r="J21" t="s">
+        <v>42</v>
+      </c>
+      <c r="U21" t="s">
         <v>42</v>
       </c>
       <c r="V21" t="s">
@@ -2156,17 +2126,14 @@
       <c r="W21" t="s">
         <v>42</v>
       </c>
-      <c r="X21" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -2176,17 +2143,17 @@
       <c r="C22" t="s">
         <v>63</v>
       </c>
+      <c r="S22" t="s">
+        <v>42</v>
+      </c>
       <c r="T22" t="s">
         <v>42</v>
       </c>
-      <c r="U22" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AK22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -2197,372 +2164,375 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
         <v>44</v>
       </c>
-      <c r="AB26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AA26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
       </c>
-      <c r="I27" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="X27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
         <v>70</v>
       </c>
-      <c r="I28" t="s">
-        <v>42</v>
-      </c>
-      <c r="P28" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ28" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>42</v>
+      </c>
+      <c r="O28" t="s">
+        <v>42</v>
+      </c>
+      <c r="X28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
         <v>71</v>
       </c>
+      <c r="O29" t="s">
+        <v>42</v>
+      </c>
       <c r="P29" t="s">
         <v>42</v>
       </c>
-      <c r="Q29" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AJ29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
         <v>72</v>
       </c>
-      <c r="I30" t="s">
-        <v>42</v>
-      </c>
-      <c r="P30" t="s">
-        <v>42</v>
-      </c>
-      <c r="T30" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK30" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>42</v>
+      </c>
+      <c r="O30" t="s">
+        <v>42</v>
+      </c>
+      <c r="S30" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
         <v>73</v>
       </c>
-      <c r="I31" t="s">
-        <v>42</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="H31" t="s">
+        <v>42</v>
+      </c>
+      <c r="O31" t="s">
+        <v>42</v>
+      </c>
+      <c r="S31" t="s">
         <v>42</v>
       </c>
       <c r="T31" t="s">
         <v>42</v>
       </c>
-      <c r="U31" t="s">
+      <c r="AJ31" t="s">
         <v>42</v>
       </c>
       <c r="AK31" t="s">
         <v>42</v>
       </c>
-      <c r="AL31" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AM31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
         <v>74</v>
       </c>
-      <c r="I32" t="s">
-        <v>42</v>
-      </c>
-      <c r="P32" t="s">
+      <c r="H32" t="s">
+        <v>42</v>
+      </c>
+      <c r="O32" t="s">
+        <v>42</v>
+      </c>
+      <c r="S32" t="s">
         <v>42</v>
       </c>
       <c r="T32" t="s">
         <v>42</v>
       </c>
-      <c r="U32" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB32" t="s">
+      <c r="AA32" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ32" t="s">
         <v>42</v>
       </c>
       <c r="AK32" t="s">
         <v>42</v>
       </c>
-      <c r="AL32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C38" t="s">
         <v>77</v>
       </c>
+      <c r="AC38" t="s">
+        <v>42</v>
+      </c>
       <c r="AD38" t="s">
         <v>42</v>
       </c>
-      <c r="AE38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
       </c>
+      <c r="AC39" t="s">
+        <v>42</v>
+      </c>
       <c r="AD39" t="s">
         <v>42</v>
       </c>
-      <c r="AE39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
         <v>81</v>
       </c>
+      <c r="S45" t="s">
+        <v>42</v>
+      </c>
       <c r="T45" t="s">
         <v>42</v>
       </c>
-      <c r="U45" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL45" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="5:40" x14ac:dyDescent="0.25">
+      <c r="AK45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="4:39" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>82</v>
+      </c>
       <c r="E58" t="s">
         <v>82</v>
       </c>
@@ -2599,7 +2569,7 @@
       <c r="P58" t="s">
         <v>82</v>
       </c>
-      <c r="Q58" t="s">
+      <c r="R58" t="s">
         <v>82</v>
       </c>
       <c r="S58" t="s">
@@ -2663,9 +2633,6 @@
         <v>82</v>
       </c>
       <c r="AM58" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN58" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>